<commit_message>
[POD-534] Rewrote tests broken by new binnable/boxable rules
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/po_import_cdr.xlsx
+++ b/spec/fixtures/files/po_import_cdr.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="po_import_cdr" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="65001"/>
 </workbook>
 </file>
@@ -103,9 +103,6 @@
     <t>Conditions</t>
   </si>
   <si>
-    <t>Test-bin</t>
-  </si>
-  <si>
     <t>CD-R</t>
   </si>
   <si>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>é Biography: Helen Gahagan Douglas, 1973-1983</t>
+  </si>
+  <si>
+    <t>test-bin</t>
   </si>
 </sst>
 </file>
@@ -994,11 +994,12 @@
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="9" max="9" width="47" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1087,13 +1088,16 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40031234567896</v>
+        <v>40000000000028</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2">
+        <v>40000000000036</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
       </c>
       <c r="E2">
         <v>40000000000002</v>
@@ -1102,69 +1106,72 @@
         <v>30000000000004</v>
       </c>
       <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>32</v>
-      </c>
-      <c r="L2" t="s">
-        <v>33</v>
       </c>
       <c r="M2">
         <v>1973</v>
       </c>
       <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
         <v>34</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
       </c>
       <c r="Q2">
         <v>5297141</v>
       </c>
       <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
         <v>36</v>
-      </c>
-      <c r="S2" t="s">
-        <v>37</v>
       </c>
       <c r="T2">
         <v>50488261</v>
       </c>
       <c r="V2" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" t="s">
         <v>38</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>39</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40031234567896</v>
+        <v>40000000000028</v>
       </c>
       <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <v>40000000000036</v>
+      </c>
+      <c r="D5" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
       </c>
       <c r="E5">
         <v>40000000000010</v>
@@ -1173,43 +1180,43 @@
         <v>30000000000012</v>
       </c>
       <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>44</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
         <v>46</v>
-      </c>
-      <c r="K5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" t="s">
-        <v>47</v>
       </c>
       <c r="M5">
         <v>1969</v>
       </c>
       <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" t="s">
         <v>48</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>49</v>
-      </c>
-      <c r="P5" t="s">
-        <v>50</v>
       </c>
       <c r="Q5">
         <v>4938795</v>
       </c>
       <c r="R5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S5" t="s">
         <v>51</v>
-      </c>
-      <c r="S5" t="s">
-        <v>52</v>
       </c>
       <c r="T5">
         <v>47794774</v>
@@ -1218,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="V5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>